<commit_message>
Test Type (add float to orchestration
</commit_message>
<xml_diff>
--- a/data/result/cleaned_data.xlsx
+++ b/data/result/cleaned_data.xlsx
@@ -653,11 +653,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Company_8</t>
+          <t>Company_9</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -665,27 +665,25 @@
           <t>Active</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Ab tt</t>
-        </is>
+      <c r="D9" t="n">
+        <v>3749.58</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>PRJ-811</t>
+          <t>PRJ-842</t>
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>46034.67946717593</v>
+        <v>46033.67946717593</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Company_9</t>
+          <t>Company_10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -694,15 +692,15 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3749.58</v>
+        <v>1729.65</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>PRJ-842</t>
+          <t>PRJ-813</t>
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>46033.67946717593</v>
+        <v>46032.67946717593</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Test Type Data type correction
</commit_message>
<xml_diff>
--- a/data/result/cleaned_data.xlsx
+++ b/data/result/cleaned_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1849,89 +1849,89 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Company_59</t>
+          <t>Company_61</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>1082.23</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>PRJ-382</t>
+          <t>PRJ-903</t>
         </is>
       </c>
       <c r="F55" s="2" t="n">
-        <v>45983.67946717593</v>
+        <v>45981.67946717593</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Company_61</t>
+          <t>Company_62</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>1082.23</v>
+        <v>4961.25</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>PRJ-903</t>
+          <t>PRJ-698</t>
         </is>
       </c>
       <c r="F56" s="2" t="n">
-        <v>45981.67946717593</v>
+        <v>45980.67946717593</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Company_62</t>
+          <t>Company_63</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>4961.25</v>
+        <v>0</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>PRJ-698</t>
+          <t>PRJ-306</t>
         </is>
       </c>
       <c r="F57" s="2" t="n">
-        <v>45980.67946717593</v>
+        <v>45979.67946717593</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Company_63</t>
+          <t>Company_64</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1944,46 +1944,46 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>PRJ-306</t>
+          <t>PRJ-734</t>
         </is>
       </c>
       <c r="F58" s="2" t="n">
-        <v>45979.67946717593</v>
+        <v>45978.67946717593</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Company_64</t>
+          <t>Company_66</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>3395.27</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>PRJ-734</t>
+          <t>PRJ-424</t>
         </is>
       </c>
       <c r="F59" s="2" t="n">
-        <v>45978.67946717593</v>
+        <v>45976.67946717593</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Company_66</t>
+          <t>Company_67</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1992,24 +1992,24 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>3395.27</v>
+        <v>3933.29</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>PRJ-424</t>
+          <t>PRJ-106</t>
         </is>
       </c>
       <c r="F60" s="2" t="n">
-        <v>45976.67946717593</v>
+        <v>45975.67946717593</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Company_67</t>
+          <t>Company_68</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2018,76 +2018,76 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>3933.29</v>
+        <v>2422.8</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>PRJ-106</t>
+          <t>PRJ-196</t>
         </is>
       </c>
       <c r="F61" s="2" t="n">
-        <v>45975.67946717593</v>
+        <v>45974.67946717593</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Company_68</t>
+          <t>Company_69</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>2422.8</v>
+        <v>0</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>PRJ-196</t>
+          <t>PRJ-583</t>
         </is>
       </c>
       <c r="F62" s="2" t="n">
-        <v>45974.67946717593</v>
+        <v>45973.67946717593</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Company_69</t>
+          <t>Company_71</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>PRJ-583</t>
+          <t>PRJ-273</t>
         </is>
       </c>
       <c r="F63" s="2" t="n">
-        <v>45973.67946717593</v>
+        <v>45971.67946717593</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Company_71</t>
+          <t>Company_72</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2096,128 +2096,128 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>4874.64</v>
+        <v>3250.33</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>PRJ-273</t>
+          <t>PRJ-366</t>
         </is>
       </c>
       <c r="F64" s="2" t="n">
-        <v>45971.67946717593</v>
+        <v>45970.67946717593</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Company_72</t>
+          <t>Company_73</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>3250.33</v>
+        <v>3602.25</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>PRJ-366</t>
+          <t>PRJ-409</t>
         </is>
       </c>
       <c r="F65" s="2" t="n">
-        <v>45970.67946717593</v>
+        <v>45969.67946717593</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Company_73</t>
+          <t>Company_74</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>3602.25</v>
+        <v>4472.66</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>PRJ-409</t>
+          <t>PRJ-790</t>
         </is>
       </c>
       <c r="F66" s="2" t="n">
-        <v>45969.67946717593</v>
+        <v>45968.67946717593</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Company_74</t>
+          <t>Company_76</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4472.66</v>
+        <v>0</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>PRJ-790</t>
+          <t>PRJ-250</t>
         </is>
       </c>
       <c r="F67" s="2" t="n">
-        <v>45968.67946717593</v>
+        <v>45966.67946717593</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Company_76</t>
+          <t>Company_77</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>1730.46</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>PRJ-250</t>
+          <t>PRJ-981</t>
         </is>
       </c>
       <c r="F68" s="2" t="n">
-        <v>45966.67946717593</v>
+        <v>45965.67946717593</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Company_77</t>
+          <t>Company_78</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2226,76 +2226,76 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>1730.46</v>
+        <v>3946.39</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>PRJ-981</t>
+          <t>PRJ-948</t>
         </is>
       </c>
       <c r="F69" s="2" t="n">
-        <v>45965.67946717593</v>
+        <v>45964.67946717593</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Company_78</t>
+          <t>sdflkjsldkfnlksdfsdflkjsdflksdlfkjsldkfjn sdvlklsdjflsjdflsjdfl sdlkhjsdlifjsldjf lisjdfoijsdf olisjdfoijsdof</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>3946.39</v>
+        <v>2710.22</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>PRJ-948</t>
+          <t>PRJ-127</t>
         </is>
       </c>
       <c r="F70" s="2" t="n">
-        <v>45964.67946717593</v>
+        <v>45963.67946717593</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Company_79</t>
+          <t>Company_80</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>2710.22</v>
+        <v>2107.11</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>PRJ-127</t>
+          <t>PRJ-437</t>
         </is>
       </c>
       <c r="F71" s="2" t="n">
-        <v>45963.67946717593</v>
+        <v>45962.67946717593</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Company_80</t>
+          <t>Company_81</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2304,76 +2304,76 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>2107.11</v>
+        <v>1389.97</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>PRJ-437</t>
+          <t>PRJ-542</t>
         </is>
       </c>
       <c r="F72" s="2" t="n">
-        <v>45962.67946717593</v>
+        <v>45961.67946717593</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Company_81</t>
+          <t>Company_82</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>1389.97</v>
+        <v>0</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>PRJ-542</t>
+          <t>PRJ-511</t>
         </is>
       </c>
       <c r="F73" s="2" t="n">
-        <v>45961.67946717593</v>
+        <v>45960.67946717593</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Company_82</t>
+          <t>Company_83</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>1914.52</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>PRJ-511</t>
+          <t>PRJ-751</t>
         </is>
       </c>
       <c r="F74" s="2" t="n">
-        <v>45960.67946717593</v>
+        <v>45959.67946717593</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Company_83</t>
+          <t>Company_84</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2382,50 +2382,50 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1914.52</v>
+        <v>2435.37</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>PRJ-751</t>
+          <t>PRJ-778</t>
         </is>
       </c>
       <c r="F75" s="2" t="n">
-        <v>45959.67946717593</v>
+        <v>45958.67946717593</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Company_84</t>
+          <t>Company_85</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>2435.37</v>
+        <v>2482.43</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>PRJ-778</t>
+          <t>PRJ-770</t>
         </is>
       </c>
       <c r="F76" s="2" t="n">
-        <v>45958.67946717593</v>
+        <v>45957.67946717593</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Company_85</t>
+          <t>Company_86</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2434,24 +2434,24 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>2482.43</v>
+        <v>1075.83</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>PRJ-770</t>
+          <t>PRJ-458</t>
         </is>
       </c>
       <c r="F77" s="2" t="n">
-        <v>45957.67946717593</v>
+        <v>45956.67946717593</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Company_86</t>
+          <t>Company_87</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2460,76 +2460,74 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>1075.83</v>
+        <v>4672.28</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>PRJ-458</t>
+          <t>PRJ-524</t>
         </is>
       </c>
       <c r="F78" s="2" t="n">
-        <v>45956.67946717593</v>
+        <v>45955.67946717593</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Company_87</t>
+          <t>Company_88</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>4672.28</v>
+        <v>0</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>PRJ-524</t>
+          <t>PRJ-303</t>
         </is>
       </c>
       <c r="F79" s="2" t="n">
-        <v>45955.67946717593</v>
+        <v>45954.67946717593</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Company_88</t>
+          <t>Company_89</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>4921.38</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>PRJ-303</t>
-        </is>
-      </c>
-      <c r="F80" s="2" t="n">
-        <v>45954.67946717593</v>
-      </c>
+          <t>PRJ-325</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Company_89</t>
+          <t>Company_91</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2538,50 +2536,50 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>4921.38</v>
+        <v>3276.87</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>PRJ-325</t>
+          <t>PRJ-331</t>
         </is>
       </c>
       <c r="F81" s="2" t="n">
-        <v>45953.67946717593</v>
+        <v>45951.67946717593</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Company_91</t>
+          <t>Company_92</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>3276.87</v>
+        <v>4512.15</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>PRJ-331</t>
+          <t>PRJ-644</t>
         </is>
       </c>
       <c r="F82" s="2" t="n">
-        <v>45951.67946717593</v>
+        <v>45950.67946717593</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Company_92</t>
+          <t>Company_93</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2590,76 +2588,76 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>4512.15</v>
+        <v>4301.01</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>PRJ-644</t>
+          <t>PRJ-710</t>
         </is>
       </c>
       <c r="F83" s="2" t="n">
-        <v>45950.67946717593</v>
+        <v>45949.67946717593</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Company_93</t>
+          <t>Company_94</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>4301.01</v>
+        <v>2085.99</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>PRJ-710</t>
+          <t>PRJ-518</t>
         </is>
       </c>
       <c r="F84" s="2" t="n">
-        <v>45949.67946717593</v>
+        <v>45948.67946717593</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Company_94</t>
+          <t>Company_96</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>2085.99</v>
+        <v>1827.61</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>PRJ-518</t>
+          <t>PRJ-340</t>
         </is>
       </c>
       <c r="F85" s="2" t="n">
-        <v>45948.67946717593</v>
+        <v>45946.67946717593</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Company_96</t>
+          <t>Company_97</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2668,76 +2666,76 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>1827.61</v>
+        <v>3441.77</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>PRJ-340</t>
+          <t>PRJ-772</t>
         </is>
       </c>
       <c r="F86" s="2" t="n">
-        <v>45946.67946717593</v>
+        <v>45945.67946717593</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Company_97</t>
+          <t>Company_98</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>3441.77</v>
+        <v>4315.01</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>PRJ-772</t>
+          <t>PRJ-538</t>
         </is>
       </c>
       <c r="F87" s="2" t="n">
-        <v>45945.67946717593</v>
+        <v>45944.67946717593</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Company_98</t>
+          <t>Company_99</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>hdh</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>4315.01</v>
+        <v>2664.09</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>PRJ-538</t>
+          <t>PRJ-961</t>
         </is>
       </c>
       <c r="F88" s="2" t="n">
-        <v>45944.67946717593</v>
+        <v>45943.67946717593</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Company_99</t>
+          <t>Company_100</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2746,24 +2744,24 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>2664.09</v>
+        <v>1912.77</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>PRJ-961</t>
+          <t>PRJ-710</t>
         </is>
       </c>
       <c r="F89" s="2" t="n">
-        <v>45943.67946717593</v>
+        <v>45942.67946717593</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Company_100</t>
+          <t>Company_101</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2772,76 +2770,76 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>1912.77</v>
+        <v>2133.09</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>PRJ-710</t>
+          <t>PRJ-567</t>
         </is>
       </c>
       <c r="F90" s="2" t="n">
-        <v>45942.67946717593</v>
+        <v>45941.67946717593</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Company_101</t>
+          <t>Company_102</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>2133.09</v>
+        <v>0</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>PRJ-567</t>
+          <t>PRJ-823</t>
         </is>
       </c>
       <c r="F91" s="2" t="n">
-        <v>45941.67946717593</v>
+        <v>45940.67946717593</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Company_102</t>
+          <t>Company_103</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>2218.85</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>PRJ-823</t>
+          <t>PRJ-139</t>
         </is>
       </c>
       <c r="F92" s="2" t="n">
-        <v>45940.67946717593</v>
+        <v>45939.67946717593</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Company_103</t>
+          <t>Company_104</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2850,180 +2848,180 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>2218.85</v>
+        <v>2431.92</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>PRJ-139</t>
+          <t>PRJ-527</t>
         </is>
       </c>
       <c r="F93" s="2" t="n">
-        <v>45939.67946717593</v>
+        <v>45938.67946717593</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Company_104</t>
+          <t>Company_106</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>2431.92</v>
+        <v>1011.63</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>PRJ-527</t>
+          <t>PRJ-900</t>
         </is>
       </c>
       <c r="F94" s="2" t="n">
-        <v>45938.67946717593</v>
+        <v>45936.67946717593</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Company_106</t>
+          <t>Company_107</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>1011.63</v>
+        <v>2950.09</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>PRJ-900</t>
+          <t>PRJ-610</t>
         </is>
       </c>
       <c r="F95" s="2" t="n">
-        <v>45936.67946717593</v>
+        <v>45935.67946717593</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Company_107</t>
+          <t>Company_108</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>2950.09</v>
+        <v>0</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>PRJ-610</t>
+          <t>PRJ-919</t>
         </is>
       </c>
       <c r="F96" s="2" t="n">
-        <v>45935.67946717593</v>
+        <v>45934.67946717593</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Company_108</t>
+          <t>Company_109</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>3558.02</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>PRJ-919</t>
+          <t>PRJ-210</t>
         </is>
       </c>
       <c r="F97" s="2" t="n">
-        <v>45934.67946717593</v>
+        <v>45933.67946717593</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Company_109</t>
+          <t>Company_110</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>3558.02</v>
+        <v>2309.16</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>PRJ-210</t>
+          <t>PRJ-517</t>
         </is>
       </c>
       <c r="F98" s="2" t="n">
-        <v>45933.67946717593</v>
+        <v>45932.67946717593</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Company_110</t>
+          <t>Company_111</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>2309.16</v>
+        <v>2150.69</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>PRJ-517</t>
+          <t>PRJ-368</t>
         </is>
       </c>
       <c r="F99" s="2" t="n">
-        <v>45932.67946717593</v>
+        <v>45931.67946717593</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Company_111</t>
+          <t>Company_112</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3032,24 +3030,24 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>2150.69</v>
+        <v>1379.48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>PRJ-368</t>
+          <t>PRJ-602</t>
         </is>
       </c>
       <c r="F100" s="2" t="n">
-        <v>45931.67946717593</v>
+        <v>45930.67946717593</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Company_112</t>
+          <t>Company_113</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3058,50 +3056,50 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>1379.48</v>
+        <v>4806.71</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>PRJ-602</t>
+          <t>PRJ-326</t>
         </is>
       </c>
       <c r="F101" s="2" t="n">
-        <v>45930.67946717593</v>
+        <v>45929.67946717593</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Company_113</t>
+          <t>Company_114</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>4806.71</v>
+        <v>3960.98</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>PRJ-326</t>
+          <t>PRJ-400</t>
         </is>
       </c>
       <c r="F102" s="2" t="n">
-        <v>45929.67946717593</v>
+        <v>45928.67946717593</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Company_114</t>
+          <t>Company_116</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3110,102 +3108,102 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>3960.98</v>
+        <v>1189.1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>PRJ-400</t>
+          <t>PRJ-590</t>
         </is>
       </c>
       <c r="F103" s="2" t="n">
-        <v>45928.67946717593</v>
+        <v>45926.67946717593</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Company_116</t>
+          <t>Company_117</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>1189.1</v>
+        <v>2642.77</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>PRJ-590</t>
+          <t>PRJ-709</t>
         </is>
       </c>
       <c r="F104" s="2" t="n">
-        <v>45926.67946717593</v>
+        <v>45925.67946717593</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Company_117</t>
+          <t>Company_118</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>2642.77</v>
+        <v>1229.35</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>PRJ-709</t>
+          <t>PRJ-880</t>
         </is>
       </c>
       <c r="F105" s="2" t="n">
-        <v>45925.67946717593</v>
+        <v>45924.67946717593</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Company_118</t>
+          <t>Company_119</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>1229.35</v>
+        <v>0</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>PRJ-880</t>
+          <t>PRJ-190</t>
         </is>
       </c>
       <c r="F106" s="2" t="n">
-        <v>45924.67946717593</v>
+        <v>45923.67946717593</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Company_119</t>
+          <t>Company_121</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3218,20 +3216,20 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>PRJ-190</t>
+          <t>PRJ-466</t>
         </is>
       </c>
       <c r="F107" s="2" t="n">
-        <v>45923.67946717593</v>
+        <v>45921.67946717593</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Company_121</t>
+          <t>Company_122</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3244,20 +3242,20 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>PRJ-466</t>
+          <t>PRJ-362</t>
         </is>
       </c>
       <c r="F108" s="2" t="n">
-        <v>45921.67946717593</v>
+        <v>45920.67946717593</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Company_122</t>
+          <t>Company_123</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3270,20 +3268,20 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>PRJ-362</t>
+          <t>PRJ-990</t>
         </is>
       </c>
       <c r="F109" s="2" t="n">
-        <v>45920.67946717593</v>
+        <v>45919.67946717593</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Company_123</t>
+          <t>Company_124</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3296,20 +3294,20 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>PRJ-990</t>
+          <t>PRJ-632</t>
         </is>
       </c>
       <c r="F110" s="2" t="n">
-        <v>45919.67946717593</v>
+        <v>45918.67946717593</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Company_124</t>
+          <t>Company_126</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3322,46 +3320,46 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>PRJ-632</t>
+          <t>PRJ-601</t>
         </is>
       </c>
       <c r="F111" s="2" t="n">
-        <v>45918.67946717593</v>
+        <v>45916.67946717593</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Company_126</t>
+          <t>Company_127</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>1773.73</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>PRJ-601</t>
+          <t>PRJ-285</t>
         </is>
       </c>
       <c r="F112" s="2" t="n">
-        <v>45916.67946717593</v>
+        <v>45915.67946717593</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Company_127</t>
+          <t>Company_128</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3370,206 +3368,206 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>1773.73</v>
+        <v>3098.39</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>PRJ-285</t>
+          <t>PRJ-138</t>
         </is>
       </c>
       <c r="F113" s="2" t="n">
-        <v>45915.67946717593</v>
+        <v>45914.67946717593</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Company_128</t>
+          <t>Company_129</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>3098.39</v>
+        <v>0</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>PRJ-138</t>
+          <t>PRJ-883</t>
         </is>
       </c>
       <c r="F114" s="2" t="n">
-        <v>45914.67946717593</v>
+        <v>45913.67946717593</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Company_129</t>
+          <t>Company_130</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>2172</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>PRJ-883</t>
+          <t>PRJ-985</t>
         </is>
       </c>
       <c r="F115" s="2" t="n">
-        <v>45913.67946717593</v>
+        <v>45912.67946717593</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Company_130</t>
+          <t>Company_131</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>2172</v>
+        <v>2920.68</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>PRJ-985</t>
+          <t>PRJ-962</t>
         </is>
       </c>
       <c r="F116" s="2" t="n">
-        <v>45912.67946717593</v>
+        <v>45911.67946717593</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Company_131</t>
+          <t>Company_132</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>2920.68</v>
+        <v>4923.31</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>PRJ-962</t>
+          <t>PRJ-484</t>
         </is>
       </c>
       <c r="F117" s="2" t="n">
-        <v>45911.67946717593</v>
+        <v>45910.67946717593</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Company_132</t>
+          <t>Company_133</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>4923.31</v>
+        <v>4534.2</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>PRJ-484</t>
+          <t>PRJ-694</t>
         </is>
       </c>
       <c r="F118" s="2" t="n">
-        <v>45910.67946717593</v>
+        <v>45909.67946717593</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Company_133</t>
+          <t>Company_134</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>4534.2</v>
+        <v>1805.47</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>PRJ-694</t>
+          <t>PRJ-823</t>
         </is>
       </c>
       <c r="F119" s="2" t="n">
-        <v>45909.67946717593</v>
+        <v>45908.67946717593</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Company_134</t>
+          <t>Company_136</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>1805.47</v>
+        <v>0</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>PRJ-823</t>
+          <t>PRJ-887</t>
         </is>
       </c>
       <c r="F120" s="2" t="n">
-        <v>45908.67946717593</v>
+        <v>45906.67946717593</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Company_136</t>
+          <t>Company_137</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3582,72 +3580,72 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>PRJ-887</t>
+          <t>PRJ-775</t>
         </is>
       </c>
       <c r="F121" s="2" t="n">
-        <v>45906.67946717593</v>
+        <v>45905.67946717593</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Company_137</t>
+          <t>Company_138</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>1564.72</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>PRJ-775</t>
+          <t>PRJ-157</t>
         </is>
       </c>
       <c r="F122" s="2" t="n">
-        <v>45905.67946717593</v>
+        <v>45904.67946717593</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Company_138</t>
+          <t>Company_139</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>1564.72</v>
+        <v>4770.43</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>PRJ-157</t>
+          <t>PRJ-354</t>
         </is>
       </c>
       <c r="F123" s="2" t="n">
-        <v>45904.67946717593</v>
+        <v>45903.67946717593</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Company_139</t>
+          <t>Company_140</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3656,154 +3654,154 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>4770.43</v>
+        <v>3772.16</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>PRJ-354</t>
+          <t>PRJ-931</t>
         </is>
       </c>
       <c r="F124" s="2" t="n">
-        <v>45903.67946717593</v>
+        <v>45902.67946717593</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Company_140</t>
+          <t>Company_141</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>3772.16</v>
+        <v>2788.09</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>PRJ-931</t>
+          <t>PRJ-968</t>
         </is>
       </c>
       <c r="F125" s="2" t="n">
-        <v>45902.67946717593</v>
+        <v>45901.67946717593</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Company_141</t>
+          <t>Company_142</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>2788.09</v>
+        <v>0</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>PRJ-968</t>
+          <t>PRJ-491</t>
         </is>
       </c>
       <c r="F126" s="2" t="n">
-        <v>45901.67946717593</v>
+        <v>45900.67946717593</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Company_142</t>
+          <t>Company_143</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>2634.27</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>PRJ-491</t>
+          <t>PRJ-576</t>
         </is>
       </c>
       <c r="F127" s="2" t="n">
-        <v>45900.67946717593</v>
+        <v>45899.67946717593</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Company_143</t>
+          <t>Company_144</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>2634.27</v>
+        <v>2403.34</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>PRJ-576</t>
+          <t>PRJ-168</t>
         </is>
       </c>
       <c r="F128" s="2" t="n">
-        <v>45899.67946717593</v>
+        <v>45898.67946717593</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Company_144</t>
+          <t>Company_146</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>2403.34</v>
+        <v>1789.68</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>PRJ-168</t>
+          <t>PRJ-523</t>
         </is>
       </c>
       <c r="F129" s="2" t="n">
-        <v>45898.67946717593</v>
+        <v>45896.67946717593</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Company_146</t>
+          <t>Company_147</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3812,24 +3810,24 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>1789.68</v>
+        <v>3558.58</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>PRJ-523</t>
+          <t>PRJ-137</t>
         </is>
       </c>
       <c r="F130" s="2" t="n">
-        <v>45896.67946717593</v>
+        <v>45895.67946717593</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Company_147</t>
+          <t>Company_148</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3838,50 +3836,50 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>3558.58</v>
+        <v>4545.67</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>PRJ-137</t>
+          <t>PRJ-989</t>
         </is>
       </c>
       <c r="F131" s="2" t="n">
-        <v>45895.67946717593</v>
+        <v>45894.67946717593</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Company_148</t>
+          <t>Company_149</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>4545.67</v>
+        <v>0</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>PRJ-989</t>
+          <t>PRJ-331</t>
         </is>
       </c>
       <c r="F132" s="2" t="n">
-        <v>45894.67946717593</v>
+        <v>45893.67946717593</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Company_149</t>
+          <t>Company_151</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3894,20 +3892,20 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>PRJ-331</t>
+          <t>PRJ-400</t>
         </is>
       </c>
       <c r="F133" s="2" t="n">
-        <v>45893.67946717593</v>
+        <v>45891.67946717593</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Company_151</t>
+          <t>Company_152</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3920,46 +3918,46 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>PRJ-400</t>
+          <t>PRJ-612</t>
         </is>
       </c>
       <c r="F134" s="2" t="n">
-        <v>45891.67946717593</v>
+        <v>45890.67946717593</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Company_152</t>
+          <t>Company_153</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>1625.78</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>PRJ-612</t>
+          <t>PRJ-895</t>
         </is>
       </c>
       <c r="F135" s="2" t="n">
-        <v>45890.67946717593</v>
+        <v>45889.67946717593</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Company_153</t>
+          <t>Company_154</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3968,50 +3966,50 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>1625.78</v>
+        <v>2716.09</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>PRJ-895</t>
+          <t>PRJ-590</t>
         </is>
       </c>
       <c r="F136" s="2" t="n">
-        <v>45889.67946717593</v>
+        <v>45888.67946717593</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Company_154</t>
+          <t>Company_156</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>2716.09</v>
+        <v>2882.55</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>PRJ-590</t>
+          <t>PRJ-193</t>
         </is>
       </c>
       <c r="F137" s="2" t="n">
-        <v>45888.67946717593</v>
+        <v>45886.67946717593</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Company_156</t>
+          <t>Company_157</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4020,102 +4018,102 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>2882.55</v>
+        <v>2487.58</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>PRJ-193</t>
+          <t>PRJ-820</t>
         </is>
       </c>
       <c r="F138" s="2" t="n">
-        <v>45886.67946717593</v>
+        <v>45885.67946717593</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Company_157</t>
+          <t>Company_158</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>2487.58</v>
+        <v>0</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>PRJ-820</t>
+          <t>PRJ-673</t>
         </is>
       </c>
       <c r="F139" s="2" t="n">
-        <v>45885.67946717593</v>
+        <v>45884.67946717593</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Company_158</t>
+          <t>Company_159</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>4406.73</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>PRJ-673</t>
+          <t>PRJ-294</t>
         </is>
       </c>
       <c r="F140" s="2" t="n">
-        <v>45884.67946717593</v>
+        <v>45883.67946717593</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Company_159</t>
+          <t>Company_160</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>4406.73</v>
+        <v>2478.67</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>PRJ-294</t>
+          <t>PRJ-920</t>
         </is>
       </c>
       <c r="F141" s="2" t="n">
-        <v>45883.67946717593</v>
+        <v>45882.67946717593</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Company_160</t>
+          <t>Company_161</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4124,50 +4122,50 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>2478.67</v>
+        <v>1619.72</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>PRJ-920</t>
+          <t>PRJ-907</t>
         </is>
       </c>
       <c r="F142" s="2" t="n">
-        <v>45882.67946717593</v>
+        <v>45881.67946717593</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Company_161</t>
+          <t>Company_162</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>1619.72</v>
+        <v>3002.62</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>PRJ-907</t>
+          <t>PRJ-314</t>
         </is>
       </c>
       <c r="F143" s="2" t="n">
-        <v>45881.67946717593</v>
+        <v>45880.67946717593</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Company_162</t>
+          <t>Company_163</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4176,24 +4174,24 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>3002.62</v>
+        <v>4129.25</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>PRJ-314</t>
+          <t>PRJ-691</t>
         </is>
       </c>
       <c r="F144" s="2" t="n">
-        <v>45880.67946717593</v>
+        <v>45879.67946717593</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Company_163</t>
+          <t>Company_164</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4202,128 +4200,128 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>4129.25</v>
+        <v>4096.61</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>PRJ-691</t>
+          <t>PRJ-693</t>
         </is>
       </c>
       <c r="F145" s="2" t="n">
-        <v>45879.67946717593</v>
+        <v>45878.67946717593</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Company_164</t>
+          <t>Company_166</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>4096.61</v>
+        <v>2919.85</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>PRJ-693</t>
+          <t>PRJ-762</t>
         </is>
       </c>
       <c r="F146" s="2" t="n">
-        <v>45878.67946717593</v>
+        <v>45876.67946717593</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Company_166</t>
+          <t>Company_167</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>2919.85</v>
+        <v>0</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>PRJ-762</t>
+          <t>PRJ-229</t>
         </is>
       </c>
       <c r="F147" s="2" t="n">
-        <v>45876.67946717593</v>
+        <v>45875.67946717593</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Company_167</t>
+          <t>Company_168</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>3323.25</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>PRJ-229</t>
+          <t>PRJ-374</t>
         </is>
       </c>
       <c r="F148" s="2" t="n">
-        <v>45875.67946717593</v>
+        <v>45874.67946717593</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Company_168</t>
+          <t>Company_169</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>3323.25</v>
+        <v>1151.37</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>PRJ-374</t>
+          <t>PRJ-733</t>
         </is>
       </c>
       <c r="F149" s="2" t="n">
-        <v>45874.67946717593</v>
+        <v>45873.67946717593</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Company_169</t>
+          <t>Company_170</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4332,76 +4330,76 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>1151.37</v>
+        <v>2901.5</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>PRJ-733</t>
+          <t>PRJ-941</t>
         </is>
       </c>
       <c r="F150" s="2" t="n">
-        <v>45873.67946717593</v>
+        <v>45872.67946717593</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Company_170</t>
+          <t>Company_171</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>2901.5</v>
+        <v>0</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>PRJ-941</t>
+          <t>PRJ-325</t>
         </is>
       </c>
       <c r="F151" s="2" t="n">
-        <v>45872.67946717593</v>
+        <v>45871.67946717593</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Company_171</t>
+          <t>Company_172</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>2847.23</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>PRJ-325</t>
+          <t>PRJ-810</t>
         </is>
       </c>
       <c r="F152" s="2" t="n">
-        <v>45871.67946717593</v>
+        <v>45870.67946717593</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Company_172</t>
+          <t>Company_173</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4410,24 +4408,24 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>2847.23</v>
+        <v>1238.17</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>PRJ-810</t>
+          <t>PRJ-736</t>
         </is>
       </c>
       <c r="F153" s="2" t="n">
-        <v>45870.67946717593</v>
+        <v>45869.67946717593</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Company_173</t>
+          <t>Company_174</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -4436,24 +4434,24 @@
         </is>
       </c>
       <c r="D154" t="n">
-        <v>1238.17</v>
+        <v>2814.06</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>PRJ-736</t>
+          <t>PRJ-767</t>
         </is>
       </c>
       <c r="F154" s="2" t="n">
-        <v>45869.67946717593</v>
+        <v>45868.67946717593</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Company_174</t>
+          <t>Company_176</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4462,50 +4460,50 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>2814.06</v>
+        <v>1519.78</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>PRJ-767</t>
+          <t>PRJ-902</t>
         </is>
       </c>
       <c r="F155" s="2" t="n">
-        <v>45868.67946717593</v>
+        <v>45866.67946717593</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Company_176</t>
+          <t>Company_177</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>1519.78</v>
+        <v>0</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>PRJ-902</t>
+          <t>PRJ-426</t>
         </is>
       </c>
       <c r="F156" s="2" t="n">
-        <v>45866.67946717593</v>
+        <v>45865.67946717593</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Company_177</t>
+          <t>Company_178</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4518,254 +4516,254 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>PRJ-426</t>
+          <t>PRJ-234</t>
         </is>
       </c>
       <c r="F157" s="2" t="n">
-        <v>45865.67946717593</v>
+        <v>45864.67946717593</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Company_178</t>
+          <t>Company_179</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>0</v>
+        <v>4364.01</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>PRJ-234</t>
+          <t>PRJ-621</t>
         </is>
       </c>
       <c r="F158" s="2" t="n">
-        <v>45864.67946717593</v>
+        <v>45863.67946717593</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Company_179</t>
+          <t>Company_181</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>4364.01</v>
+        <v>0</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>PRJ-621</t>
+          <t>PRJ-198</t>
         </is>
       </c>
       <c r="F159" s="2" t="n">
-        <v>45863.67946717593</v>
+        <v>45861.67946717593</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Company_181</t>
+          <t>Company_182</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>1653.44</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>PRJ-198</t>
+          <t>PRJ-117</t>
         </is>
       </c>
       <c r="F160" s="2" t="n">
-        <v>45861.67946717593</v>
+        <v>45860.67946717593</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Company_182</t>
+          <t>Company_183</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>1653.44</v>
+        <v>0</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>PRJ-117</t>
+          <t>PRJ-462</t>
         </is>
       </c>
       <c r="F161" s="2" t="n">
-        <v>45860.67946717593</v>
+        <v>45859.67946717593</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Company_183</t>
+          <t>Company_184</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>3778.51</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>PRJ-462</t>
+          <t>PRJ-260</t>
         </is>
       </c>
       <c r="F162" s="2" t="n">
-        <v>45859.67946717593</v>
+        <v>45858.67946717593</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Company_184</t>
+          <t>Company_186</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>3778.51</v>
+        <v>0</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>PRJ-260</t>
+          <t>PRJ-993</t>
         </is>
       </c>
       <c r="F163" s="2" t="n">
-        <v>45858.67946717593</v>
+        <v>45856.67946717593</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Company_186</t>
+          <t>Company_187</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>1759.35</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>PRJ-993</t>
+          <t>PRJ-837</t>
         </is>
       </c>
       <c r="F164" s="2" t="n">
-        <v>45856.67946717593</v>
+        <v>45855.67946717593</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Company_187</t>
+          <t>Company_188</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>1759.35</v>
+        <v>2139.08</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>PRJ-837</t>
+          <t>PRJ-230</t>
         </is>
       </c>
       <c r="F165" s="2" t="n">
-        <v>45855.67946717593</v>
+        <v>45854.67946717593</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Company_188</t>
+          <t>Company_189</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>2139.08</v>
+        <v>0</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>PRJ-230</t>
+          <t>PRJ-777</t>
         </is>
       </c>
       <c r="F166" s="2" t="n">
-        <v>45854.67946717593</v>
+        <v>45853.67946717593</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>1189</v>
+        <v>1191</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Company_189</t>
+          <t>Company_191</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -4778,46 +4776,46 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>PRJ-777</t>
+          <t>PRJ-178</t>
         </is>
       </c>
       <c r="F167" s="2" t="n">
-        <v>45853.67946717593</v>
+        <v>45851.67946717593</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Company_191</t>
+          <t>Company_192</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>2224.85</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>PRJ-178</t>
+          <t>PRJ-868</t>
         </is>
       </c>
       <c r="F168" s="2" t="n">
-        <v>45851.67946717593</v>
+        <v>45850.67946717593</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Company_192</t>
+          <t>Company_193</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4826,170 +4824,144 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>2224.85</v>
+        <v>2196.71</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>PRJ-868</t>
+          <t>PRJ-867</t>
         </is>
       </c>
       <c r="F169" s="2" t="n">
-        <v>45850.67946717593</v>
+        <v>45849.67946717593</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Company_193</t>
+          <t>Company_194</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>2196.71</v>
+        <v>0</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>PRJ-867</t>
+          <t>PRJ-292</t>
         </is>
       </c>
       <c r="F170" s="2" t="n">
-        <v>45849.67946717593</v>
+        <v>45848.67946717593</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Company_194</t>
+          <t>Company_196</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>0</v>
+        <v>1538.48</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>PRJ-292</t>
+          <t>PRJ-576</t>
         </is>
       </c>
       <c r="F171" s="2" t="n">
-        <v>45848.67946717593</v>
+        <v>45846.67946717593</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Company_196</t>
+          <t>Company_197</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Deactive</t>
+          <t>Suspend</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>1538.48</v>
+        <v>0</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>PRJ-576</t>
+          <t>PRJ-839</t>
         </is>
       </c>
       <c r="F172" s="2" t="n">
-        <v>45846.67946717593</v>
+        <v>45845.67946717593</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Company_197</t>
+          <t>Company_198</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Suspend</t>
+          <t>Active</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>0</v>
+        <v>1333.26</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>PRJ-839</t>
+          <t>PRJ-330</t>
         </is>
       </c>
       <c r="F173" s="2" t="n">
-        <v>45845.67946717593</v>
+        <v>45844.67946717593</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Company_198</t>
+          <t>Company_199</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Deactive</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>1333.26</v>
+        <v>3108.68</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>PRJ-330</t>
+          <t>PRJ-702</t>
         </is>
       </c>
       <c r="F174" s="2" t="n">
-        <v>45844.67946717593</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="n">
-        <v>1199</v>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>Company_199</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Deactive</t>
-        </is>
-      </c>
-      <c r="D175" t="n">
-        <v>3108.68</v>
-      </c>
-      <c r="E175" t="inlineStr">
-        <is>
-          <t>PRJ-702</t>
-        </is>
-      </c>
-      <c r="F175" s="2" t="n">
         <v>45843.67946717593</v>
       </c>
     </row>

</xml_diff>